<commit_message>
fix: update API doc
</commit_message>
<xml_diff>
--- a/_docs/REST API.xlsx
+++ b/_docs/REST API.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="93">
   <si>
     <t>Emergency Release</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -47,10 +47,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[name, favorate, enable, x, y, rotation]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>[name, x, y, rotation]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -84,14 +80,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/map/scan/start</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/map/scan/stop</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>GET</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -104,10 +92,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/map/${name}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/map</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -275,9 +259,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[name, favorate, enable, x, y, rotation]</t>
-  </si>
-  <si>
     <t>로딩 / 준비 / 주행 / 긴급정지</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -291,10 +272,6 @@
   </si>
   <si>
     <t>/robot/jog</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>즉시 멈춤</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -382,6 +359,35 @@
 로봇설정, map, 거점, 가상벽 등
 모든 정보 포함됨</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/schedule</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스케줄</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>즉시 멈춤</t>
+  </si>
+  <si>
+    <t>/robot/mode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/map/scan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/map/content</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[name, favorite, enable, x, y, rotation]</t>
   </si>
 </sst>
 </file>
@@ -428,7 +434,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -612,13 +618,89 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -649,47 +731,86 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -992,328 +1113,330 @@
     <row r="1" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="2:7" ht="26.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="16" t="s">
+      <c r="B3" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="22"/>
+      <c r="D3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="F3" s="16"/>
-      <c r="G3" s="17"/>
+      <c r="E3" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" s="10"/>
+      <c r="G3" s="11"/>
     </row>
     <row r="4" spans="2:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="19"/>
-      <c r="C4" s="13"/>
+      <c r="C4" s="20"/>
       <c r="D4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="2:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="19"/>
-      <c r="C5" s="13"/>
+      <c r="C5" s="20"/>
       <c r="D5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="5"/>
     </row>
     <row r="6" spans="2:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="19"/>
-      <c r="C6" s="13"/>
+      <c r="C6" s="20"/>
       <c r="D6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="19"/>
-      <c r="C7" s="13"/>
+      <c r="C7" s="20"/>
       <c r="D7" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="19"/>
-      <c r="C8" s="13"/>
+      <c r="C8" s="20"/>
       <c r="D8" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="5" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="19"/>
-      <c r="C9" s="13"/>
+      <c r="C9" s="20"/>
       <c r="D9" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>3</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="19"/>
-      <c r="C10" s="13"/>
+      <c r="C10" s="20"/>
       <c r="D10" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="2:7" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="20"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="3" t="s">
+    <row r="11" spans="2:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="34"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="E11" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="35"/>
+      <c r="G11" s="36" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="16"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E12" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F12" s="3"/>
+      <c r="G12" s="6"/>
+    </row>
+    <row r="13" spans="2:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" s="26"/>
+      <c r="D13" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14" spans="2:7" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="32"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="3"/>
-      <c r="G11" s="6" t="s">
+      <c r="F14" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" s="28"/>
+      <c r="D15" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="F15" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="G15" s="30" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="32"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="12" spans="2:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="G12" s="7"/>
-    </row>
-    <row r="13" spans="2:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="19"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="2" t="s">
+      <c r="E16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" s="6"/>
+    </row>
+    <row r="17" spans="2:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" s="17"/>
+      <c r="D17" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="16"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="19"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E14" s="2" t="s">
+      <c r="E18" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="20"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G15" s="6"/>
-    </row>
-    <row r="16" spans="2:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E16" s="4" t="s">
+      <c r="F18" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="G18" s="6"/>
+    </row>
+    <row r="19" spans="2:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19" s="17"/>
+      <c r="D19" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G16" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="20"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G17" s="6"/>
-    </row>
-    <row r="18" spans="2:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="4" t="s">
+      <c r="E19" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="19"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" s="2" t="s">
+      <c r="F19" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F19" s="2"/>
-      <c r="G19" s="5" t="s">
-        <v>23</v>
+      <c r="G19" s="7" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="19"/>
-      <c r="C20" s="13"/>
+      <c r="C20" s="20"/>
       <c r="D20" s="2" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F20" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F20" s="2"/>
+      <c r="G20" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="19"/>
-      <c r="C21" s="13"/>
+      <c r="C21" s="20"/>
       <c r="D21" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E21" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="2"/>
       <c r="G21" s="5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="20"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="3" t="s">
+      <c r="B22" s="19"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F22" s="3"/>
-      <c r="G22" s="6"/>
+      <c r="E22" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F22" s="2"/>
+      <c r="G22" s="5" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="23" spans="2:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="21" t="s">
-        <v>87</v>
+      <c r="B23" s="15" t="s">
+        <v>81</v>
       </c>
       <c r="C23" s="23" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="7"/>
@@ -1325,7 +1448,7 @@
         <v>2</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="5"/>
@@ -1337,56 +1460,58 @@
         <v>2</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="2:7" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="20"/>
-      <c r="C26" s="20"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
       <c r="D26" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="2:7" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="12"/>
+      <c r="B27" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="C12:C15"/>
-    <mergeCell ref="B3:B11"/>
-    <mergeCell ref="C3:C11"/>
+  <mergeCells count="13">
     <mergeCell ref="C23:C26"/>
     <mergeCell ref="B23:B26"/>
-    <mergeCell ref="B18:B22"/>
-    <mergeCell ref="C18:C22"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="C19:C22"/>
     <mergeCell ref="C27:G27"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="B3:B12"/>
+    <mergeCell ref="C3:C12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="C15:C16"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -1411,29 +1536,29 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
         <v>51</v>
-      </c>
-      <c r="C2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
@@ -1441,86 +1566,86 @@
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D14" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C18" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D18" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D20" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>